<commit_message>
modify some nonstandard code
</commit_message>
<xml_diff>
--- a/easyexcel-test/src/test/resources/demo/demo.xlsx
+++ b/easyexcel-test/src/test/resources/demo/demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowHeight="17020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t>字符串标题</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>字符串1</t>
-  </si>
-  <si>
-    <t>字符串2</t>
   </si>
   <si>
     <t>字符串3</t>
@@ -91,10 +88,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -105,9 +102,115 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,76 +224,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -199,51 +241,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,13 +255,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,13 +405,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,67 +417,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,79 +435,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,6 +446,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -484,48 +529,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -535,17 +538,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,152 +551,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -708,58 +705,61 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1055,19 +1055,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="11.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="17.8333333333333" customWidth="1"/>
-    <col min="3" max="3" width="11.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.3365384615385" customWidth="1"/>
+    <col min="2" max="2" width="17.8365384615385" customWidth="1"/>
+    <col min="3" max="3" width="11.3365384615385" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
@@ -1104,9 +1104,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="2">
         <v>43833.0423726852</v>
       </c>
@@ -1116,7 +1114,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>43834.0423726852</v>
@@ -1127,7 +1125,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>43835.0423726852</v>
@@ -1138,7 +1136,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>43836.0423726852</v>
@@ -1149,7 +1147,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>43837.0423726852</v>
@@ -1160,7 +1158,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>43838.0423726852</v>
@@ -1171,7 +1169,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>43839.0423726852</v>
@@ -1182,7 +1180,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>43840.0423726852</v>
@@ -1192,14 +1190,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A4"/>
+  </mergeCells>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1207,7 +1208,7 @@
       <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1222,7 +1223,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>43831.0423726852</v>
@@ -1233,7 +1234,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>43832.0423726852</v>
@@ -1244,7 +1245,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>43833.0423726852</v>
@@ -1255,7 +1256,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>43834.0423726852</v>
@@ -1266,7 +1267,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>43835.0423726852</v>
@@ -1277,7 +1278,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>43836.0423726852</v>
@@ -1288,7 +1289,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>43837.0423726852</v>
@@ -1299,7 +1300,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>43838.0423726852</v>
@@ -1310,7 +1311,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>43839.0423726852</v>
@@ -1321,7 +1322,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>43840.0423726852</v>

</xml_diff>